<commit_message>
added photos, changed some colors
</commit_message>
<xml_diff>
--- a/album_pages/descriptions.xlsx
+++ b/album_pages/descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quiana/Documents/Projects/qstodder.github.io/album_pages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547C0690-BA11-8542-B0D1-E39C7B462E8F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9524205-6CF6-B840-B4A6-625C112F0603}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13620" yWindow="460" windowWidth="15180" windowHeight="16640" xr2:uid="{0F25ED81-FF29-D94A-9429-46818CDE6378}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>title</t>
   </si>
@@ -120,12 +120,6 @@
     <t>desc_color</t>
   </si>
   <si>
-    <t>grey</t>
-  </si>
-  <si>
-    <t>Some Good 'Ol Bishop Climbing</t>
-  </si>
-  <si>
     <t>Alabama Hills (in the shadow of Mt Whitney), The Happies, The Sads, and much more</t>
   </si>
   <si>
@@ -172,13 +166,90 @@
   </si>
   <si>
     <t>Round Town</t>
+  </si>
+  <si>
+    <t>rgb(90, 88, 88)</t>
+  </si>
+  <si>
+    <t>rgb(163, 201, 133)</t>
+  </si>
+  <si>
+    <t>Some Good 'Ol Bishop/Lone Pine Climbing</t>
+  </si>
+  <si>
+    <r>
+      <t>rgb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>229</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>230</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>173</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -190,6 +261,36 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFDCDCAA"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -213,10 +314,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA0DFF7-88C9-324C-86E3-C11E9246E750}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,7 +654,7 @@
         <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -581,8 +685,8 @@
       <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>29</v>
+      <c r="F2" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -599,24 +703,24 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
@@ -627,8 +731,8 @@
       <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
+      <c r="F4" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -638,8 +742,8 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
+      <c r="B5" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>23</v>
@@ -650,8 +754,8 @@
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>29</v>
+      <c r="F5" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -673,8 +777,8 @@
       <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>29</v>
+      <c r="F6" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -696,8 +800,8 @@
       <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>29</v>
+      <c r="F7" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G7" t="s">
         <v>19</v>
@@ -714,13 +818,13 @@
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>29</v>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G8" t="s">
         <v>21</v>
@@ -742,16 +846,16 @@
       <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
+      <c r="F9" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -760,21 +864,21 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>29</v>
+      <c r="F10" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -783,21 +887,21 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>29</v>
+      <c r="F11" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -806,21 +910,21 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>29</v>
+      <c r="F12" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -829,16 +933,16 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>29</v>
+      <c r="F13" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>